<commit_message>
separado nombre en nombre y apellidos del profesor
</commit_message>
<xml_diff>
--- a/web_app/data/infoProf.xlsx
+++ b/web_app/data/infoProf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG-PAP\docs_iniciales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TFG\TFG-PAP\web_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB76E1-7971-4055-B293-A1EA2557C842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC930BD-E38A-4F63-926B-23D0119E753F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="990" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="orden" sheetId="3" r:id="rId1"/>
@@ -1131,9 +1131,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1171,7 +1171,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1277,7 +1277,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1419,7 +1419,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1427,20 +1427,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F730222-8754-E042-AC44-B395574E42F1}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.875" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="41.8984375" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1450,8 +1450,12 @@
       <c r="C1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="str">
+        <f>PROPER(B1)</f>
+        <v>Toro Bonilla, Jose Miguel</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1461,8 +1465,12 @@
       <c r="C2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" si="0">PROPER(B2)</f>
+        <v>Riquelme Santos, Jose Cristobal</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1472,8 +1480,12 @@
       <c r="C3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>Ortega Ramirez, Juan Antonio</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1483,8 +1495,12 @@
       <c r="C4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>Ruiz Cortes, Antonio</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1494,8 +1510,12 @@
       <c r="C5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>Escalona Cuaresma, Maria Jose</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1505,8 +1525,12 @@
       <c r="C6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>Martinez Gasca, Rafael</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -1516,8 +1540,12 @@
       <c r="C7" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Benavides Cuevas, David Felipe</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1527,8 +1555,12 @@
       <c r="C8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Gomez Lopez, Maria Teresa</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1538,8 +1570,12 @@
       <c r="C9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Ruiz Cortes, David</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1549,8 +1585,12 @@
       <c r="C10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>Resinas Arias De Reyna, Manuel</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1560,8 +1600,12 @@
       <c r="C11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>Segura Rueda, Sergio</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1571,8 +1615,12 @@
       <c r="C12" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>Mejias Risoto, Manuel</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1582,8 +1630,12 @@
       <c r="C13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>Troyano Jimenez, Jose Antonio</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1593,8 +1645,12 @@
       <c r="C14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>Torres Valderrama, Jesus</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1604,8 +1660,12 @@
       <c r="C15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>Gonzalez Romano, Jose Mariano</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1615,8 +1675,12 @@
       <c r="C16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>Corchuelo Gil, Rafael</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1626,8 +1690,12 @@
       <c r="C17" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>Galan Morillo, Francisco Jose</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1637,8 +1705,12 @@
       <c r="C18" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>Diaz Madrigal, Victor Jesus</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1648,8 +1720,12 @@
       <c r="C19" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>Duran Toro, Amador</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1659,8 +1735,12 @@
       <c r="C20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>Valle Sevillano, Carmelo Del</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1670,8 +1750,12 @@
       <c r="C21" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>Perez Castellanos, Jose Antonio</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1681,8 +1765,12 @@
       <c r="C22" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>Romero Aleta, Rafael</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1692,8 +1780,12 @@
       <c r="C23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>Carrillo Montero, Vicente</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1703,8 +1795,12 @@
       <c r="C24" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>Cordero Valle, Juan Manuel</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1714,8 +1810,12 @@
       <c r="C25" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>Cañete Valdeon, Jose Miguel</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1725,8 +1825,12 @@
       <c r="C26" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>Rubio Escudero, Cristina</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1736,8 +1840,12 @@
       <c r="C27" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>Alvarez Garcia, Juan Antonio</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1747,8 +1855,12 @@
       <c r="C28" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>Fernandez-Montes Gonzalez, Alejandro</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1758,8 +1870,12 @@
       <c r="C29" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>Barba Rodriguez, Irene</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1769,8 +1885,12 @@
       <c r="C30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>Parejo Maestre, José Antonio</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1780,8 +1900,12 @@
       <c r="C31" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>Ortega Rodriguez, Francisco Javier</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>32</v>
       </c>
@@ -1791,8 +1915,12 @@
       <c r="C32" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Nepomuceno Chamorro, Isabel De Los Angeles</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>33</v>
       </c>
@@ -1802,8 +1930,12 @@
       <c r="C33" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Cruz Mata, Fermin</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>34</v>
       </c>
@@ -1813,8 +1945,12 @@
       <c r="C34" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Martinez Ballesteros, Maria Del Mar</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>35</v>
       </c>
@@ -1824,8 +1960,12 @@
       <c r="C35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Trinidad Martin-Arroyo, Pablo</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>36</v>
       </c>
@@ -1835,8 +1975,12 @@
       <c r="C36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Dominguez Mayo, Francisco Jose</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -1846,8 +1990,12 @@
       <c r="C37" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Garcia Gutierrez, Jorge</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>38</v>
       </c>
@@ -1857,8 +2005,12 @@
       <c r="C38" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Garcia Rodriguez, Jose M.</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>39</v>
       </c>
@@ -1868,8 +2020,12 @@
       <c r="C39" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Hernandez Salmeron, Inmaculada Concepción</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>40</v>
       </c>
@@ -1879,8 +2035,12 @@
       <c r="C40" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Fernandez Montes, Pablo</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>41</v>
       </c>
@@ -1890,8 +2050,12 @@
       <c r="C41" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Enriquez De Salamanca Ros, Fernando</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>42</v>
       </c>
@@ -1901,8 +2065,12 @@
       <c r="C42" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Rio Ortega, Adela Del</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>43</v>
       </c>
@@ -1912,8 +2080,12 @@
       <c r="C43" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Soria Morillo, Luis Miguel</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>44</v>
       </c>
@@ -1923,8 +2095,12 @@
       <c r="C44" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Galindo Duarte, José Ángel</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>45</v>
       </c>
@@ -1934,8 +2110,12 @@
       <c r="C45" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Varela Vaca, Angel Jesus</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>46</v>
       </c>
@@ -1945,8 +2125,12 @@
       <c r="C46" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Müller Cejas, Carlos Guillermo</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>47</v>
       </c>
@@ -1956,8 +2140,12 @@
       <c r="C47" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Marquez Chamorro, Alfonso Eduardo</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>48</v>
       </c>
@@ -1967,8 +2155,12 @@
       <c r="C48" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>Arevalo Maldonado, Carlos</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>49</v>
       </c>
@@ -1978,8 +2170,12 @@
       <c r="C49" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>Romero Moreno, Luisa Maria</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>50</v>
       </c>
@@ -1989,8 +2185,12 @@
       <c r="C50" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>Cruz Risco, Maria Margarita</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>51</v>
       </c>
@@ -2000,8 +2200,12 @@
       <c r="C51" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>Jimenez Ramirez, Andres</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>52</v>
       </c>
@@ -2011,8 +2215,12 @@
       <c r="C52" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>Fernandez Cerero, Damian</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>53</v>
       </c>
@@ -2022,8 +2230,12 @@
       <c r="C53" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>Cabanillas Macias, Cristina</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>54</v>
       </c>
@@ -2033,8 +2245,12 @@
       <c r="C54" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>Jimenez Aguirre, Patricia</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>55</v>
       </c>
@@ -2044,8 +2260,12 @@
       <c r="C55" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>González Enríquez, José</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>56</v>
       </c>
@@ -2055,8 +2275,12 @@
       <c r="C56" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>Peña Siles, Joaquin</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>57</v>
       </c>
@@ -2066,8 +2290,12 @@
       <c r="C57" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>Martin Diaz, Octavio</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>58</v>
       </c>
@@ -2077,8 +2305,12 @@
       <c r="C58" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>Bernardez Jimenez, Beatriz</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>59</v>
       </c>
@@ -2088,8 +2320,12 @@
       <c r="C59" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>Neira Ayuso, Pablo</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>60</v>
       </c>
@@ -2099,8 +2335,12 @@
       <c r="C60" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>Reina Quintero, Antonia Maria</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>61</v>
       </c>
@@ -2110,8 +2350,12 @@
       <c r="C61" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>Pontes Balanza, Beatriz</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>62</v>
       </c>
@@ -2121,8 +2365,12 @@
       <c r="C62" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>Mateos Garcia, Daniel</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>63</v>
       </c>
@@ -2132,8 +2380,12 @@
       <c r="C63" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>Ceballos Guerrero, Rafael</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>64</v>
       </c>
@@ -2143,8 +2395,12 @@
       <c r="C64" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>Nepomuceno Chamorro, Juan Antonio</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>65</v>
       </c>
@@ -2154,8 +2410,12 @@
       <c r="C65" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>Gutierrez Rodriguez, Javier Jesus</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>66</v>
       </c>
@@ -2165,8 +2425,12 @@
       <c r="C66" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D89" si="1">PROPER(B66)</f>
+        <v>García García, Julián Alberto</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>67</v>
       </c>
@@ -2176,8 +2440,12 @@
       <c r="C67" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>Ferrer Troyano, Francisco Javier</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>68</v>
       </c>
@@ -2187,8 +2455,12 @@
       <c r="C68" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>Rosa Troyano, Francisco Fernando</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>69</v>
       </c>
@@ -2198,8 +2470,12 @@
       <c r="C69" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>Borrego Nuñez, Diana</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>70</v>
       </c>
@@ -2209,8 +2485,12 @@
       <c r="C70" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>Sánchez Jerez, Ana Belén</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>71</v>
       </c>
@@ -2220,8 +2500,12 @@
       <c r="C71" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>Estrada Torres, Irene Bedilia</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>72</v>
       </c>
@@ -2231,8 +2515,12 @@
       <c r="C72" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>Acuña Garrido, María Dolores De</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>73</v>
       </c>
@@ -2242,8 +2530,12 @@
       <c r="C73" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>Bengoa Diaz, Alfonso Maria De</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>74</v>
       </c>
@@ -2253,8 +2545,12 @@
       <c r="C74" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>Ayala Hernández, Daniel</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>75</v>
       </c>
@@ -2264,8 +2560,12 @@
       <c r="C75" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>Gutiérrez Avilés, David</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>76</v>
       </c>
@@ -2275,8 +2575,12 @@
       <c r="C76" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>Luna Romera, Jose Maria</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>77</v>
       </c>
@@ -2286,8 +2590,12 @@
       <c r="C77" s="2" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>Olivero, Miguél Ángel</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>78</v>
       </c>
@@ -2297,8 +2605,12 @@
       <c r="C78" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>Vega Marquez, Belen</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>79</v>
       </c>
@@ -2308,8 +2620,12 @@
       <c r="C79" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>Carranza Garcia, Manuel</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -2319,8 +2635,12 @@
       <c r="C80" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>Ramos Gutierrez, Belen</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>81</v>
       </c>
@@ -2330,8 +2650,12 @@
       <c r="C81" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>Jimenez Navarro, Manuel Jesús</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>82</v>
       </c>
@@ -2341,8 +2665,12 @@
       <c r="C82" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>Sanchez Gomez, Nicolas</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>83</v>
       </c>
@@ -2352,8 +2680,12 @@
       <c r="C83" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>Alonso Valenzuela, Juan Carlos</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>84</v>
       </c>
@@ -2363,8 +2695,12 @@
       <c r="C84" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>Bravo Llanos, Alfonso</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>85</v>
       </c>
@@ -2374,8 +2710,12 @@
       <c r="C85" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>Salas Urbano, Maria</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>86</v>
       </c>
@@ -2385,8 +2725,12 @@
       <c r="C86" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>Romero Organvidez, David</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>87</v>
       </c>
@@ -2396,8 +2740,12 @@
       <c r="C87" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>Fresno Aranda, Rafael</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>88</v>
       </c>
@@ -2407,8 +2755,12 @@
       <c r="C88" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>Martínez Rojas, Antonio</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>89</v>
       </c>
@@ -2418,8 +2770,12 @@
       <c r="C89" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>Capitan Agudo, Carlos</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C90" s="1"/>
     </row>
   </sheetData>

</xml_diff>